<commit_message>
Updating standings and knock-out teams with June 21st results
Signed-off-by: beedoug2000 <bernadette_douglas2000@hotmail.com>
</commit_message>
<xml_diff>
--- a/Euro2020/result_files/EC_2020.xlsx
+++ b/Euro2020/result_files/EC_2020.xlsx
@@ -1731,7 +1731,7 @@
   <dimension ref="B2:U65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1808,7 +1808,7 @@
         </is>
       </c>
       <c r="H5" s="11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I5" s="3" t="n"/>
       <c r="J5" s="83" t="n"/>
@@ -1818,7 +1818,7 @@
         </is>
       </c>
       <c r="L5" s="15" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -1848,7 +1848,7 @@
         </is>
       </c>
       <c r="L6" s="15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="H8" s="13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="3" t="n"/>
       <c r="J8" s="83" t="n"/>
@@ -2337,7 +2337,11 @@
           <t>Austria</t>
         </is>
       </c>
-      <c r="M24" s="88" t="n"/>
+      <c r="M24" s="88" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="C25" s="50" t="inlineStr">
@@ -2382,7 +2386,11 @@
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="M25" s="88" t="n"/>
+      <c r="M25" s="88" t="inlineStr">
+        <is>
+          <t>0-3</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="C26" s="52" t="n"/>
@@ -2415,7 +2423,11 @@
           <t>Belgium</t>
         </is>
       </c>
-      <c r="M26" s="86" t="n"/>
+      <c r="M26" s="86" t="inlineStr">
+        <is>
+          <t>0-2</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="C27" s="55" t="inlineStr">
@@ -2460,7 +2472,11 @@
           <t>Denmark</t>
         </is>
       </c>
-      <c r="M27" s="86" t="n"/>
+      <c r="M27" s="86" t="inlineStr">
+        <is>
+          <t>1-4</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="C28" s="53" t="inlineStr">
@@ -2908,7 +2924,7 @@
       <c r="B44" s="203" t="n"/>
       <c r="C44" s="200" t="inlineStr">
         <is>
-          <t>2nd Group C</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="D44" s="203" t="n"/>
@@ -2945,7 +2961,7 @@
       </c>
       <c r="C46" s="38" t="inlineStr">
         <is>
-          <t>Winner Group B</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="D46" s="202" t="n"/>
@@ -3216,7 +3232,7 @@
       </c>
       <c r="C61" s="38" t="inlineStr">
         <is>
-          <t>Winner GroupC</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D61" s="202" t="n"/>
@@ -3273,7 +3289,7 @@
       <c r="B65" s="203" t="n"/>
       <c r="C65" s="200" t="inlineStr">
         <is>
-          <t>2nd Group B</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D65" s="203" t="n"/>
@@ -3403,11 +3419,11 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Srich</t>
+          <t>Justin</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
@@ -3424,7 +3440,7 @@
         </is>
       </c>
       <c r="I3" s="11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J3" s="3" t="n"/>
       <c r="K3" s="14" t="inlineStr">
@@ -3433,17 +3449,17 @@
         </is>
       </c>
       <c r="L3" s="15" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Srich</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
@@ -3469,7 +3485,7 @@
         </is>
       </c>
       <c r="L4" s="15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -3479,7 +3495,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
@@ -3524,7 +3540,7 @@
         </is>
       </c>
       <c r="I6" s="13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J6" s="3" t="n"/>
       <c r="K6" s="16" t="inlineStr">
@@ -3724,8 +3740,8 @@
     <col width="4.140625" customWidth="1" style="217" min="14" max="14"/>
     <col width="16.7109375" customWidth="1" style="217" min="15" max="17"/>
     <col width="8.7109375" customWidth="1" style="217" min="18" max="26"/>
-    <col width="14.42578125" customWidth="1" style="217" min="27" max="32"/>
-    <col width="14.42578125" customWidth="1" style="217" min="33" max="16384"/>
+    <col width="14.42578125" customWidth="1" style="217" min="27" max="34"/>
+    <col width="14.42578125" customWidth="1" style="217" min="35" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="26.25" customHeight="1" s="191">
@@ -4934,7 +4950,7 @@
       <c r="B44" s="211" t="n"/>
       <c r="C44" s="173" t="inlineStr">
         <is>
-          <t>2nd Group C</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="D44" s="211" t="n"/>
@@ -4988,7 +5004,7 @@
       </c>
       <c r="C46" s="172" t="inlineStr">
         <is>
-          <t>Winner Group B</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="D46" s="212" t="n"/>
@@ -5299,7 +5315,7 @@
       </c>
       <c r="C61" s="172" t="inlineStr">
         <is>
-          <t>Winner GroupC</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D61" s="212" t="n"/>
@@ -5356,7 +5372,7 @@
       <c r="B65" s="211" t="n"/>
       <c r="C65" s="173" t="inlineStr">
         <is>
-          <t>2nd Group B</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D65" s="211" t="n"/>
@@ -6376,8 +6392,8 @@
     <col width="4.140625" customWidth="1" style="217" min="14" max="14"/>
     <col width="16.7109375" customWidth="1" style="217" min="15" max="17"/>
     <col width="8.7109375" customWidth="1" style="217" min="18" max="26"/>
-    <col width="14.42578125" customWidth="1" style="217" min="27" max="32"/>
-    <col width="14.42578125" customWidth="1" style="217" min="33" max="16384"/>
+    <col width="14.42578125" customWidth="1" style="217" min="27" max="34"/>
+    <col width="14.42578125" customWidth="1" style="217" min="35" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="26.25" customHeight="1" s="191">
@@ -7586,7 +7602,7 @@
       <c r="B44" s="211" t="n"/>
       <c r="C44" s="173" t="inlineStr">
         <is>
-          <t>2nd Group C</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="D44" s="211" t="n"/>
@@ -7640,7 +7656,7 @@
       </c>
       <c r="C46" s="172" t="inlineStr">
         <is>
-          <t>Winner Group B</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="D46" s="212" t="n"/>
@@ -7951,7 +7967,7 @@
       </c>
       <c r="C61" s="172" t="inlineStr">
         <is>
-          <t>Winner GroupC</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D61" s="212" t="n"/>
@@ -8008,7 +8024,7 @@
       <c r="B65" s="211" t="n"/>
       <c r="C65" s="173" t="inlineStr">
         <is>
-          <t>2nd Group B</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D65" s="211" t="n"/>
@@ -10179,7 +10195,7 @@
       <c r="B44" s="203" t="n"/>
       <c r="C44" s="200" t="inlineStr">
         <is>
-          <t>2nd Group C</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="D44" s="203" t="n"/>
@@ -10216,7 +10232,7 @@
       </c>
       <c r="C46" s="38" t="inlineStr">
         <is>
-          <t>Winner Group B</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="D46" s="202" t="n"/>
@@ -10487,7 +10503,7 @@
       </c>
       <c r="C61" s="38" t="inlineStr">
         <is>
-          <t>Winner GroupC</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D61" s="202" t="n"/>
@@ -10544,7 +10560,7 @@
       <c r="B65" s="203" t="n"/>
       <c r="C65" s="200" t="inlineStr">
         <is>
-          <t>2nd Group B</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="D65" s="203" t="n"/>

</xml_diff>

<commit_message>
Adding Lina's predictions for Round of 16
Signed-off-by: beedoug2000 <bernadette_douglas2000@hotmail.com>
</commit_message>
<xml_diff>
--- a/Euro2020/result_files/EC_2020.xlsx
+++ b/Euro2020/result_files/EC_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lina\git\Euro2020\Euro2020\result_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BC414D-CBDF-43C8-BBE7-57313B5A8494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED97BD44-43A2-4BE0-B70B-08802830A92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="100">
   <si>
     <t xml:space="preserve">EURO 2020 </t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>3-3</t>
+  </si>
+  <si>
+    <t>2-3</t>
   </si>
 </sst>
 </file>
@@ -1529,51 +1532,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="31" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="31" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="32" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1604,22 +1623,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="22" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="32" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="32" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1952,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1971,18 +1974,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="208" t="s">
+      <c r="C2" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" s="77" t="s">
@@ -2249,73 +2252,73 @@
       <c r="L15" s="83"/>
     </row>
     <row r="16" spans="3:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="D16" s="196"/>
+      <c r="E16" s="196"/>
+      <c r="F16" s="196"/>
+      <c r="G16" s="196"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="196"/>
+      <c r="J16" s="196"/>
+      <c r="K16" s="196"/>
+      <c r="L16" s="196"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="209"/>
-      <c r="E17" s="204"/>
-      <c r="F17" s="204"/>
-      <c r="G17" s="205"/>
-      <c r="H17" s="203" t="s">
+      <c r="D17" s="192"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="194"/>
+      <c r="H17" s="199" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="204"/>
-      <c r="J17" s="204"/>
-      <c r="K17" s="204"/>
-      <c r="L17" s="205"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="193"/>
+      <c r="L17" s="194"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="196"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
+      <c r="D18" s="195"/>
+      <c r="E18" s="196"/>
+      <c r="F18" s="196"/>
       <c r="G18" s="197"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="193"/>
-      <c r="J18" s="193"/>
-      <c r="K18" s="193"/>
+      <c r="H18" s="200"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="196"/>
+      <c r="K18" s="196"/>
       <c r="L18" s="197"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="3:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="207" t="s">
+      <c r="C20" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="204"/>
+      <c r="D20" s="193"/>
       <c r="E20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="36"/>
-      <c r="G20" s="207" t="s">
+      <c r="G20" s="201" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="204"/>
+      <c r="H20" s="193"/>
       <c r="I20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="J20" s="36"/>
-      <c r="K20" s="207" t="s">
+      <c r="K20" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="204"/>
+      <c r="L20" s="193"/>
       <c r="M20" s="35" t="s">
         <v>37</v>
       </c>
@@ -2745,47 +2748,47 @@
       <c r="M36" s="92"/>
     </row>
     <row r="38" spans="2:21" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="192" t="s">
+      <c r="C38" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="193"/>
-      <c r="E38" s="193"/>
-      <c r="F38" s="193"/>
-      <c r="G38" s="193"/>
-      <c r="H38" s="193"/>
-      <c r="I38" s="193"/>
-      <c r="J38" s="193"/>
-      <c r="K38" s="193"/>
-      <c r="L38" s="193"/>
+      <c r="D38" s="196"/>
+      <c r="E38" s="196"/>
+      <c r="F38" s="196"/>
+      <c r="G38" s="196"/>
+      <c r="H38" s="196"/>
+      <c r="I38" s="196"/>
+      <c r="J38" s="196"/>
+      <c r="K38" s="196"/>
+      <c r="L38" s="196"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="209"/>
-      <c r="E39" s="204"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="205"/>
-      <c r="H39" s="203" t="s">
+      <c r="D39" s="192"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="194"/>
+      <c r="H39" s="199" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="204"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="205"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
+      <c r="K39" s="193"/>
+      <c r="L39" s="194"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="196"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="193"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="196"/>
+      <c r="F40" s="196"/>
       <c r="G40" s="197"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="193"/>
-      <c r="J40" s="193"/>
-      <c r="K40" s="193"/>
+      <c r="H40" s="200"/>
+      <c r="I40" s="196"/>
+      <c r="J40" s="196"/>
+      <c r="K40" s="196"/>
       <c r="L40" s="197"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
@@ -2793,10 +2796,10 @@
       <c r="C41" s="186"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B42" s="198" t="s">
+      <c r="B42" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="193"/>
+      <c r="C42" s="196"/>
       <c r="D42" s="30" t="s">
         <v>37</v>
       </c>
@@ -2825,73 +2828,73 @@
         <v>37</v>
       </c>
       <c r="Q42" s="39"/>
-      <c r="S42" s="201"/>
-      <c r="T42" s="202"/>
+      <c r="S42" s="198"/>
+      <c r="T42" s="191"/>
       <c r="U42" s="39"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B43" s="190" t="s">
+      <c r="B43" s="207" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="195"/>
+      <c r="D43" s="202"/>
     </row>
     <row r="44" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="191"/>
+      <c r="B44" s="203"/>
       <c r="C44" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="191"/>
+      <c r="D44" s="203"/>
       <c r="E44" s="44"/>
-      <c r="F44" s="194" t="s">
+      <c r="F44" s="206" t="s">
         <v>63</v>
       </c>
       <c r="G44" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="195"/>
+      <c r="H44" s="202"/>
     </row>
     <row r="45" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="D45" s="93"/>
       <c r="E45" s="43"/>
-      <c r="F45" s="191"/>
+      <c r="F45" s="203"/>
       <c r="G45" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="191"/>
+      <c r="H45" s="203"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B46" s="190" t="s">
+      <c r="B46" s="207" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="195"/>
+      <c r="D46" s="202"/>
       <c r="G46" s="1"/>
       <c r="H46" s="94"/>
     </row>
     <row r="47" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="191"/>
+      <c r="B47" s="203"/>
       <c r="C47" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="191"/>
+      <c r="D47" s="203"/>
       <c r="G47" s="1"/>
       <c r="H47" s="95"/>
       <c r="I47" s="43"/>
-      <c r="J47" s="199" t="s">
+      <c r="J47" s="204" t="s">
         <v>67</v>
       </c>
       <c r="K47" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="L47" s="195"/>
-      <c r="S47" s="201"/>
-      <c r="T47" s="202"/>
+      <c r="L47" s="202"/>
+      <c r="S47" s="198"/>
+      <c r="T47" s="191"/>
       <c r="U47" s="39"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
@@ -2899,39 +2902,39 @@
       <c r="D48" s="93"/>
       <c r="G48" s="1"/>
       <c r="H48" s="95"/>
-      <c r="J48" s="191"/>
+      <c r="J48" s="203"/>
       <c r="K48" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L48" s="191"/>
+      <c r="L48" s="203"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="190" t="s">
+      <c r="B49" s="207" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="195"/>
+      <c r="D49" s="202"/>
       <c r="G49" s="1"/>
       <c r="H49" s="96"/>
       <c r="K49" s="37"/>
       <c r="L49" s="94"/>
     </row>
     <row r="50" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="191"/>
+      <c r="B50" s="203"/>
       <c r="C50" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="191"/>
+      <c r="D50" s="203"/>
       <c r="E50" s="43"/>
-      <c r="F50" s="194" t="s">
+      <c r="F50" s="206" t="s">
         <v>71</v>
       </c>
       <c r="G50" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H50" s="195"/>
+      <c r="H50" s="202"/>
       <c r="K50" s="37"/>
       <c r="L50" s="95"/>
     </row>
@@ -2939,50 +2942,50 @@
       <c r="B51" s="5"/>
       <c r="D51" s="93"/>
       <c r="E51" s="43"/>
-      <c r="F51" s="191"/>
+      <c r="F51" s="203"/>
       <c r="G51" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="191"/>
+      <c r="H51" s="203"/>
       <c r="K51" s="37"/>
       <c r="L51" s="95"/>
     </row>
     <row r="52" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="190" t="s">
+      <c r="B52" s="207" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="195"/>
+      <c r="D52" s="202"/>
       <c r="G52" s="1"/>
       <c r="H52" s="93"/>
       <c r="K52" s="37"/>
       <c r="L52" s="95"/>
       <c r="M52" s="43"/>
-      <c r="N52" s="200" t="s">
+      <c r="N52" s="205" t="s">
         <v>75</v>
       </c>
       <c r="O52" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="P52" s="195"/>
+      <c r="P52" s="202"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="191"/>
+      <c r="B53" s="203"/>
       <c r="C53" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="191"/>
+      <c r="D53" s="203"/>
       <c r="G53" s="1"/>
       <c r="H53" s="93"/>
       <c r="K53" s="37"/>
       <c r="L53" s="95"/>
-      <c r="N53" s="191"/>
+      <c r="N53" s="203"/>
       <c r="O53" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="P53" s="191"/>
+      <c r="P53" s="203"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
@@ -2993,32 +2996,32 @@
       <c r="L54" s="95"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="190" t="s">
+      <c r="B55" s="207" t="s">
         <v>78</v>
       </c>
       <c r="C55" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="195"/>
+      <c r="D55" s="202"/>
       <c r="G55" s="1"/>
       <c r="H55" s="93"/>
       <c r="K55" s="37"/>
       <c r="L55" s="95"/>
     </row>
     <row r="56" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="191"/>
+      <c r="B56" s="203"/>
       <c r="C56" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="191"/>
+      <c r="D56" s="203"/>
       <c r="E56" s="44"/>
-      <c r="F56" s="194" t="s">
+      <c r="F56" s="206" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="H56" s="195"/>
+      <c r="H56" s="202"/>
       <c r="K56" s="37"/>
       <c r="L56" s="95"/>
     </row>
@@ -3026,129 +3029,119 @@
       <c r="B57" s="5"/>
       <c r="D57" s="93"/>
       <c r="E57" s="45"/>
-      <c r="F57" s="191"/>
+      <c r="F57" s="203"/>
       <c r="G57" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="H57" s="191"/>
+      <c r="H57" s="203"/>
       <c r="K57" s="37"/>
       <c r="L57" s="95"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="190" t="s">
+      <c r="B58" s="207" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="195"/>
+      <c r="D58" s="202"/>
       <c r="G58" s="1"/>
       <c r="H58" s="94"/>
       <c r="K58" s="37"/>
       <c r="L58" s="96"/>
     </row>
     <row r="59" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="191"/>
+      <c r="B59" s="203"/>
       <c r="C59" s="187" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="191"/>
+      <c r="D59" s="203"/>
       <c r="G59" s="1"/>
       <c r="H59" s="95"/>
       <c r="I59" s="43"/>
-      <c r="J59" s="199" t="s">
+      <c r="J59" s="204" t="s">
         <v>83</v>
       </c>
       <c r="K59" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="L59" s="195"/>
+      <c r="L59" s="202"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="D60" s="93"/>
       <c r="G60" s="1"/>
       <c r="H60" s="95"/>
-      <c r="J60" s="191"/>
+      <c r="J60" s="203"/>
       <c r="K60" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="L60" s="191"/>
+      <c r="L60" s="203"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="190" t="s">
+      <c r="B61" s="207" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="195"/>
+      <c r="D61" s="202"/>
       <c r="G61" s="1"/>
       <c r="H61" s="96"/>
     </row>
     <row r="62" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="191"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="191"/>
+      <c r="D62" s="203"/>
       <c r="E62" s="44"/>
-      <c r="F62" s="194" t="s">
+      <c r="F62" s="206" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="H62" s="195"/>
+      <c r="H62" s="202"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="5"/>
       <c r="D63" s="93"/>
       <c r="E63" s="45"/>
-      <c r="F63" s="191"/>
+      <c r="F63" s="203"/>
       <c r="G63" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="191"/>
+      <c r="H63" s="203"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="190" t="s">
+      <c r="B64" s="207" t="s">
         <v>90</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="195"/>
+      <c r="D64" s="202"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="191"/>
+      <c r="B65" s="203"/>
       <c r="C65" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="191"/>
+      <c r="D65" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="H17:L18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="H39:L40"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C38:L38"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="F62:F63"/>
     <mergeCell ref="F56:F57"/>
     <mergeCell ref="F50:F51"/>
@@ -3164,16 +3157,26 @@
     <mergeCell ref="D61:D62"/>
     <mergeCell ref="D64:D65"/>
     <mergeCell ref="D58:D59"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C38:L38"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="H17:L18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="H39:L40"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="S42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3486,18 +3489,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="212" t="s">
+      <c r="C2" s="218" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
+      <c r="I2" s="217"/>
+      <c r="J2" s="217"/>
+      <c r="K2" s="217"/>
+      <c r="L2" s="217"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4" s="98" t="s">
@@ -3716,48 +3719,48 @@
       <c r="L15" s="100"/>
     </row>
     <row r="16" spans="3:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="213" t="s">
+      <c r="C16" s="219" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="214"/>
-      <c r="G16" s="214"/>
-      <c r="H16" s="214"/>
-      <c r="I16" s="214"/>
-      <c r="J16" s="214"/>
-      <c r="K16" s="214"/>
-      <c r="L16" s="214"/>
+      <c r="D16" s="220"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
+      <c r="K16" s="220"/>
+      <c r="L16" s="220"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C17" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="215"/>
-      <c r="E17" s="216"/>
-      <c r="F17" s="216"/>
-      <c r="G17" s="217"/>
-      <c r="H17" s="218" t="s">
+      <c r="D17" s="221"/>
+      <c r="E17" s="222"/>
+      <c r="F17" s="222"/>
+      <c r="G17" s="223"/>
+      <c r="H17" s="224" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="216"/>
-      <c r="J17" s="216"/>
-      <c r="K17" s="216"/>
-      <c r="L17" s="217"/>
+      <c r="I17" s="222"/>
+      <c r="J17" s="222"/>
+      <c r="K17" s="222"/>
+      <c r="L17" s="223"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C18" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="221"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="220"/>
+      <c r="D18" s="227"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="226"/>
+      <c r="H18" s="225"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="220"/>
+      <c r="L18" s="226"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C19" s="100"/>
@@ -3765,26 +3768,26 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="138"/>
       <c r="B20" s="138"/>
-      <c r="C20" s="222" t="s">
+      <c r="C20" s="228" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="216"/>
+      <c r="D20" s="222"/>
       <c r="E20" s="139" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="188"/>
-      <c r="G20" s="222" t="s">
+      <c r="G20" s="228" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="216"/>
+      <c r="H20" s="222"/>
       <c r="I20" s="139" t="s">
         <v>37</v>
       </c>
       <c r="J20" s="188"/>
-      <c r="K20" s="222" t="s">
+      <c r="K20" s="228" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="216"/>
+      <c r="L20" s="222"/>
       <c r="M20" s="139" t="s">
         <v>37</v>
       </c>
@@ -4254,58 +4257,58 @@
     </row>
     <row r="37" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="213" t="s">
+      <c r="C38" s="219" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="214"/>
-      <c r="E38" s="214"/>
-      <c r="F38" s="214"/>
-      <c r="G38" s="214"/>
-      <c r="H38" s="214"/>
-      <c r="I38" s="214"/>
-      <c r="J38" s="214"/>
-      <c r="K38" s="214"/>
-      <c r="L38" s="214"/>
+      <c r="D38" s="220"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="215"/>
-      <c r="E39" s="216"/>
-      <c r="F39" s="216"/>
-      <c r="G39" s="217"/>
-      <c r="H39" s="218" t="s">
+      <c r="D39" s="221"/>
+      <c r="E39" s="222"/>
+      <c r="F39" s="222"/>
+      <c r="G39" s="223"/>
+      <c r="H39" s="224" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="216"/>
-      <c r="J39" s="216"/>
-      <c r="K39" s="216"/>
-      <c r="L39" s="217"/>
+      <c r="I39" s="222"/>
+      <c r="J39" s="222"/>
+      <c r="K39" s="222"/>
+      <c r="L39" s="223"/>
     </row>
     <row r="40" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="221"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="214"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="219"/>
-      <c r="I40" s="214"/>
-      <c r="J40" s="214"/>
-      <c r="K40" s="214"/>
-      <c r="L40" s="220"/>
+      <c r="D40" s="227"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="226"/>
+      <c r="H40" s="225"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="226"/>
     </row>
     <row r="41" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="168"/>
       <c r="C41" s="169"/>
     </row>
     <row r="42" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="223" t="s">
+      <c r="B42" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="214"/>
+      <c r="C42" s="220"/>
       <c r="D42" s="170" t="s">
         <v>37</v>
       </c>
@@ -4335,19 +4338,19 @@
       </c>
       <c r="Q42" s="138"/>
       <c r="R42" s="171"/>
-      <c r="S42" s="210"/>
-      <c r="T42" s="211"/>
+      <c r="S42" s="216"/>
+      <c r="T42" s="217"/>
       <c r="U42" s="138"/>
       <c r="V42" s="171"/>
     </row>
     <row r="43" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="224" t="s">
+      <c r="B43" s="210" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="226"/>
+      <c r="D43" s="212"/>
       <c r="E43" s="171"/>
       <c r="F43" s="171"/>
       <c r="O43" s="171"/>
@@ -4360,19 +4363,19 @@
       <c r="V43" s="171"/>
     </row>
     <row r="44" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="225"/>
+      <c r="B44" s="211"/>
       <c r="C44" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="225"/>
+      <c r="D44" s="211"/>
       <c r="E44" s="174"/>
-      <c r="F44" s="227" t="s">
+      <c r="F44" s="214" t="s">
         <v>63</v>
       </c>
       <c r="G44" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="226"/>
+      <c r="H44" s="212"/>
       <c r="O44" s="171"/>
       <c r="P44" s="171"/>
       <c r="Q44" s="171"/>
@@ -4387,11 +4390,11 @@
       <c r="C45" s="171"/>
       <c r="D45" s="176"/>
       <c r="E45" s="177"/>
-      <c r="F45" s="225"/>
+      <c r="F45" s="211"/>
       <c r="G45" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="225"/>
+      <c r="H45" s="211"/>
       <c r="O45" s="171"/>
       <c r="P45" s="171"/>
       <c r="Q45" s="171"/>
@@ -4402,13 +4405,13 @@
       <c r="V45" s="171"/>
     </row>
     <row r="46" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="224" t="s">
+      <c r="B46" s="210" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="226"/>
+      <c r="D46" s="212"/>
       <c r="E46" s="171"/>
       <c r="F46" s="171"/>
       <c r="G46" s="179"/>
@@ -4423,29 +4426,29 @@
       <c r="V46" s="171"/>
     </row>
     <row r="47" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="225"/>
+      <c r="B47" s="211"/>
       <c r="C47" s="173" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="225"/>
+      <c r="D47" s="211"/>
       <c r="E47" s="171"/>
       <c r="F47" s="171"/>
       <c r="G47" s="179"/>
       <c r="H47" s="181"/>
       <c r="I47" s="177"/>
-      <c r="J47" s="228" t="s">
+      <c r="J47" s="213" t="s">
         <v>67</v>
       </c>
       <c r="K47" s="182" t="s">
         <v>68</v>
       </c>
-      <c r="L47" s="226"/>
+      <c r="L47" s="212"/>
       <c r="O47" s="171"/>
       <c r="P47" s="171"/>
       <c r="Q47" s="171"/>
       <c r="R47" s="171"/>
-      <c r="S47" s="210"/>
-      <c r="T47" s="211"/>
+      <c r="S47" s="216"/>
+      <c r="T47" s="217"/>
       <c r="U47" s="138"/>
       <c r="V47" s="171"/>
     </row>
@@ -4457,11 +4460,11 @@
       <c r="F48" s="171"/>
       <c r="G48" s="179"/>
       <c r="H48" s="181"/>
-      <c r="J48" s="225"/>
+      <c r="J48" s="211"/>
       <c r="K48" s="165" t="s">
         <v>69</v>
       </c>
-      <c r="L48" s="225"/>
+      <c r="L48" s="211"/>
       <c r="O48" s="171"/>
       <c r="P48" s="171"/>
       <c r="Q48" s="171"/>
@@ -4472,13 +4475,13 @@
       <c r="V48" s="171"/>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="224" t="s">
+      <c r="B49" s="210" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="226"/>
+      <c r="D49" s="212"/>
       <c r="E49" s="171"/>
       <c r="F49" s="171"/>
       <c r="G49" s="179"/>
@@ -4487,19 +4490,19 @@
       <c r="L49" s="180"/>
     </row>
     <row r="50" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="225"/>
+      <c r="B50" s="211"/>
       <c r="C50" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="225"/>
+      <c r="D50" s="211"/>
       <c r="E50" s="177"/>
-      <c r="F50" s="227" t="s">
+      <c r="F50" s="214" t="s">
         <v>71</v>
       </c>
       <c r="G50" s="175" t="s">
         <v>72</v>
       </c>
-      <c r="H50" s="226"/>
+      <c r="H50" s="212"/>
       <c r="K50" s="143"/>
       <c r="L50" s="181"/>
     </row>
@@ -4508,22 +4511,22 @@
       <c r="C51" s="171"/>
       <c r="D51" s="176"/>
       <c r="E51" s="177"/>
-      <c r="F51" s="225"/>
+      <c r="F51" s="211"/>
       <c r="G51" s="178" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="225"/>
+      <c r="H51" s="211"/>
       <c r="K51" s="143"/>
       <c r="L51" s="181"/>
     </row>
     <row r="52" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="224" t="s">
+      <c r="B52" s="210" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="172" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="226"/>
+      <c r="D52" s="212"/>
       <c r="E52" s="171"/>
       <c r="F52" s="171"/>
       <c r="G52" s="179"/>
@@ -4531,31 +4534,31 @@
       <c r="K52" s="143"/>
       <c r="L52" s="181"/>
       <c r="M52" s="177"/>
-      <c r="N52" s="229" t="s">
+      <c r="N52" s="215" t="s">
         <v>75</v>
       </c>
       <c r="O52" s="182" t="s">
         <v>76</v>
       </c>
-      <c r="P52" s="226"/>
+      <c r="P52" s="212"/>
     </row>
     <row r="53" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="225"/>
+      <c r="B53" s="211"/>
       <c r="C53" s="173" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="225"/>
+      <c r="D53" s="211"/>
       <c r="E53" s="171"/>
       <c r="F53" s="171"/>
       <c r="G53" s="179"/>
       <c r="H53" s="176"/>
       <c r="K53" s="143"/>
       <c r="L53" s="181"/>
-      <c r="N53" s="225"/>
+      <c r="N53" s="211"/>
       <c r="O53" s="165" t="s">
         <v>77</v>
       </c>
-      <c r="P53" s="225"/>
+      <c r="P53" s="211"/>
     </row>
     <row r="54" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="138"/>
@@ -4569,13 +4572,13 @@
       <c r="L54" s="181"/>
     </row>
     <row r="55" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="224" t="s">
+      <c r="B55" s="210" t="s">
         <v>78</v>
       </c>
       <c r="C55" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="226"/>
+      <c r="D55" s="212"/>
       <c r="E55" s="171"/>
       <c r="F55" s="171"/>
       <c r="G55" s="179"/>
@@ -4584,19 +4587,19 @@
       <c r="L55" s="181"/>
     </row>
     <row r="56" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="225"/>
+      <c r="B56" s="211"/>
       <c r="C56" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="225"/>
+      <c r="D56" s="211"/>
       <c r="E56" s="174"/>
-      <c r="F56" s="227" t="s">
+      <c r="F56" s="214" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="H56" s="226"/>
+      <c r="H56" s="212"/>
       <c r="K56" s="143"/>
       <c r="L56" s="181"/>
     </row>
@@ -4604,106 +4607,106 @@
       <c r="B57" s="138"/>
       <c r="D57" s="176"/>
       <c r="E57" s="184"/>
-      <c r="F57" s="225"/>
+      <c r="F57" s="211"/>
       <c r="G57" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="H57" s="225"/>
+      <c r="H57" s="211"/>
       <c r="K57" s="143"/>
       <c r="L57" s="181"/>
     </row>
     <row r="58" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="224" t="s">
+      <c r="B58" s="210" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="226"/>
+      <c r="D58" s="212"/>
       <c r="G58" s="179"/>
       <c r="H58" s="180"/>
       <c r="K58" s="143"/>
       <c r="L58" s="183"/>
     </row>
     <row r="59" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="225"/>
+      <c r="B59" s="211"/>
       <c r="C59" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="225"/>
+      <c r="D59" s="211"/>
       <c r="G59" s="179"/>
       <c r="H59" s="181"/>
       <c r="I59" s="177"/>
-      <c r="J59" s="228" t="s">
+      <c r="J59" s="213" t="s">
         <v>83</v>
       </c>
       <c r="K59" s="182" t="s">
         <v>84</v>
       </c>
-      <c r="L59" s="226"/>
+      <c r="L59" s="212"/>
     </row>
     <row r="60" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="138"/>
       <c r="D60" s="176"/>
       <c r="G60" s="179"/>
       <c r="H60" s="181"/>
-      <c r="J60" s="225"/>
+      <c r="J60" s="211"/>
       <c r="K60" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="L60" s="225"/>
+      <c r="L60" s="211"/>
     </row>
     <row r="61" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="224" t="s">
+      <c r="B61" s="210" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="226"/>
+      <c r="D61" s="212"/>
       <c r="G61" s="179"/>
       <c r="H61" s="183"/>
     </row>
     <row r="62" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="225"/>
+      <c r="B62" s="211"/>
       <c r="C62" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="225"/>
+      <c r="D62" s="211"/>
       <c r="E62" s="174"/>
-      <c r="F62" s="227" t="s">
+      <c r="F62" s="214" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="H62" s="226"/>
+      <c r="H62" s="212"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="138"/>
       <c r="D63" s="176"/>
       <c r="E63" s="184"/>
-      <c r="F63" s="225"/>
+      <c r="F63" s="211"/>
       <c r="G63" s="178" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="225"/>
+      <c r="H63" s="211"/>
     </row>
     <row r="64" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="224" t="s">
+      <c r="B64" s="210" t="s">
         <v>90</v>
       </c>
       <c r="C64" s="172" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="226"/>
+      <c r="D64" s="212"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="225"/>
+      <c r="B65" s="211"/>
       <c r="C65" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="225"/>
+      <c r="D65" s="211"/>
     </row>
     <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5642,37 +5645,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C16:L16"/>
@@ -5687,6 +5659,37 @@
     <mergeCell ref="H39:L40"/>
     <mergeCell ref="D40:G40"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="J59:J60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5719,18 +5722,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="212" t="s">
+      <c r="C2" s="218" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
+      <c r="I2" s="217"/>
+      <c r="J2" s="217"/>
+      <c r="K2" s="217"/>
+      <c r="L2" s="217"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4" s="98" t="s">
@@ -5949,48 +5952,48 @@
       <c r="L15" s="100"/>
     </row>
     <row r="16" spans="3:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="213" t="s">
+      <c r="C16" s="219" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="214"/>
-      <c r="G16" s="214"/>
-      <c r="H16" s="214"/>
-      <c r="I16" s="214"/>
-      <c r="J16" s="214"/>
-      <c r="K16" s="214"/>
-      <c r="L16" s="214"/>
+      <c r="D16" s="220"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="220"/>
+      <c r="H16" s="220"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
+      <c r="K16" s="220"/>
+      <c r="L16" s="220"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C17" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="215"/>
-      <c r="E17" s="216"/>
-      <c r="F17" s="216"/>
-      <c r="G17" s="217"/>
-      <c r="H17" s="218" t="s">
+      <c r="D17" s="221"/>
+      <c r="E17" s="222"/>
+      <c r="F17" s="222"/>
+      <c r="G17" s="223"/>
+      <c r="H17" s="224" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="216"/>
-      <c r="J17" s="216"/>
-      <c r="K17" s="216"/>
-      <c r="L17" s="217"/>
+      <c r="I17" s="222"/>
+      <c r="J17" s="222"/>
+      <c r="K17" s="222"/>
+      <c r="L17" s="223"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C18" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="221"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="220"/>
+      <c r="D18" s="227"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="220"/>
+      <c r="G18" s="226"/>
+      <c r="H18" s="225"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="220"/>
+      <c r="L18" s="226"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C19" s="100"/>
@@ -5998,26 +6001,26 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="138"/>
       <c r="B20" s="138"/>
-      <c r="C20" s="222" t="s">
+      <c r="C20" s="228" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="216"/>
+      <c r="D20" s="222"/>
       <c r="E20" s="139" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="188"/>
-      <c r="G20" s="222" t="s">
+      <c r="G20" s="228" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="216"/>
+      <c r="H20" s="222"/>
       <c r="I20" s="139" t="s">
         <v>37</v>
       </c>
       <c r="J20" s="188"/>
-      <c r="K20" s="222" t="s">
+      <c r="K20" s="228" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="216"/>
+      <c r="L20" s="222"/>
       <c r="M20" s="139" t="s">
         <v>37</v>
       </c>
@@ -6487,58 +6490,58 @@
     </row>
     <row r="37" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="213" t="s">
+      <c r="C38" s="219" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="214"/>
-      <c r="E38" s="214"/>
-      <c r="F38" s="214"/>
-      <c r="G38" s="214"/>
-      <c r="H38" s="214"/>
-      <c r="I38" s="214"/>
-      <c r="J38" s="214"/>
-      <c r="K38" s="214"/>
-      <c r="L38" s="214"/>
+      <c r="D38" s="220"/>
+      <c r="E38" s="220"/>
+      <c r="F38" s="220"/>
+      <c r="G38" s="220"/>
+      <c r="H38" s="220"/>
+      <c r="I38" s="220"/>
+      <c r="J38" s="220"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="220"/>
     </row>
     <row r="39" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="215"/>
-      <c r="E39" s="216"/>
-      <c r="F39" s="216"/>
-      <c r="G39" s="217"/>
-      <c r="H39" s="218" t="s">
+      <c r="D39" s="221"/>
+      <c r="E39" s="222"/>
+      <c r="F39" s="222"/>
+      <c r="G39" s="223"/>
+      <c r="H39" s="224" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="216"/>
-      <c r="J39" s="216"/>
-      <c r="K39" s="216"/>
-      <c r="L39" s="217"/>
+      <c r="I39" s="222"/>
+      <c r="J39" s="222"/>
+      <c r="K39" s="222"/>
+      <c r="L39" s="223"/>
     </row>
     <row r="40" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="221"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="214"/>
-      <c r="G40" s="220"/>
-      <c r="H40" s="219"/>
-      <c r="I40" s="214"/>
-      <c r="J40" s="214"/>
-      <c r="K40" s="214"/>
-      <c r="L40" s="220"/>
+      <c r="D40" s="227"/>
+      <c r="E40" s="220"/>
+      <c r="F40" s="220"/>
+      <c r="G40" s="226"/>
+      <c r="H40" s="225"/>
+      <c r="I40" s="220"/>
+      <c r="J40" s="220"/>
+      <c r="K40" s="220"/>
+      <c r="L40" s="226"/>
     </row>
     <row r="41" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="168"/>
       <c r="C41" s="169"/>
     </row>
     <row r="42" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="223" t="s">
+      <c r="B42" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="214"/>
+      <c r="C42" s="220"/>
       <c r="D42" s="170" t="s">
         <v>37</v>
       </c>
@@ -6568,19 +6571,19 @@
       </c>
       <c r="Q42" s="138"/>
       <c r="R42" s="171"/>
-      <c r="S42" s="210"/>
-      <c r="T42" s="211"/>
+      <c r="S42" s="216"/>
+      <c r="T42" s="217"/>
       <c r="U42" s="138"/>
       <c r="V42" s="171"/>
     </row>
     <row r="43" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="224" t="s">
+      <c r="B43" s="210" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="226"/>
+      <c r="D43" s="212"/>
       <c r="E43" s="171"/>
       <c r="F43" s="171"/>
       <c r="O43" s="171"/>
@@ -6593,19 +6596,19 @@
       <c r="V43" s="171"/>
     </row>
     <row r="44" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="225"/>
+      <c r="B44" s="211"/>
       <c r="C44" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="225"/>
+      <c r="D44" s="211"/>
       <c r="E44" s="174"/>
-      <c r="F44" s="227" t="s">
+      <c r="F44" s="214" t="s">
         <v>63</v>
       </c>
       <c r="G44" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="226"/>
+      <c r="H44" s="212"/>
       <c r="O44" s="171"/>
       <c r="P44" s="171"/>
       <c r="Q44" s="171"/>
@@ -6620,11 +6623,11 @@
       <c r="C45" s="171"/>
       <c r="D45" s="176"/>
       <c r="E45" s="177"/>
-      <c r="F45" s="225"/>
+      <c r="F45" s="211"/>
       <c r="G45" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="225"/>
+      <c r="H45" s="211"/>
       <c r="O45" s="171"/>
       <c r="P45" s="171"/>
       <c r="Q45" s="171"/>
@@ -6635,13 +6638,13 @@
       <c r="V45" s="171"/>
     </row>
     <row r="46" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="224" t="s">
+      <c r="B46" s="210" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="226"/>
+      <c r="D46" s="212"/>
       <c r="E46" s="171"/>
       <c r="F46" s="171"/>
       <c r="G46" s="179"/>
@@ -6656,29 +6659,29 @@
       <c r="V46" s="171"/>
     </row>
     <row r="47" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="225"/>
+      <c r="B47" s="211"/>
       <c r="C47" s="173" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="225"/>
+      <c r="D47" s="211"/>
       <c r="E47" s="171"/>
       <c r="F47" s="171"/>
       <c r="G47" s="179"/>
       <c r="H47" s="181"/>
       <c r="I47" s="177"/>
-      <c r="J47" s="228" t="s">
+      <c r="J47" s="213" t="s">
         <v>67</v>
       </c>
       <c r="K47" s="182" t="s">
         <v>68</v>
       </c>
-      <c r="L47" s="226"/>
+      <c r="L47" s="212"/>
       <c r="O47" s="171"/>
       <c r="P47" s="171"/>
       <c r="Q47" s="171"/>
       <c r="R47" s="171"/>
-      <c r="S47" s="210"/>
-      <c r="T47" s="211"/>
+      <c r="S47" s="216"/>
+      <c r="T47" s="217"/>
       <c r="U47" s="138"/>
       <c r="V47" s="171"/>
     </row>
@@ -6690,11 +6693,11 @@
       <c r="F48" s="171"/>
       <c r="G48" s="179"/>
       <c r="H48" s="181"/>
-      <c r="J48" s="225"/>
+      <c r="J48" s="211"/>
       <c r="K48" s="165" t="s">
         <v>69</v>
       </c>
-      <c r="L48" s="225"/>
+      <c r="L48" s="211"/>
       <c r="O48" s="171"/>
       <c r="P48" s="171"/>
       <c r="Q48" s="171"/>
@@ -6705,13 +6708,13 @@
       <c r="V48" s="171"/>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="224" t="s">
+      <c r="B49" s="210" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="226"/>
+      <c r="D49" s="212"/>
       <c r="E49" s="171"/>
       <c r="F49" s="171"/>
       <c r="G49" s="179"/>
@@ -6720,19 +6723,19 @@
       <c r="L49" s="180"/>
     </row>
     <row r="50" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="225"/>
+      <c r="B50" s="211"/>
       <c r="C50" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="225"/>
+      <c r="D50" s="211"/>
       <c r="E50" s="177"/>
-      <c r="F50" s="227" t="s">
+      <c r="F50" s="214" t="s">
         <v>71</v>
       </c>
       <c r="G50" s="175" t="s">
         <v>72</v>
       </c>
-      <c r="H50" s="226"/>
+      <c r="H50" s="212"/>
       <c r="K50" s="143"/>
       <c r="L50" s="181"/>
     </row>
@@ -6741,22 +6744,22 @@
       <c r="C51" s="171"/>
       <c r="D51" s="176"/>
       <c r="E51" s="177"/>
-      <c r="F51" s="225"/>
+      <c r="F51" s="211"/>
       <c r="G51" s="178" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="225"/>
+      <c r="H51" s="211"/>
       <c r="K51" s="143"/>
       <c r="L51" s="181"/>
     </row>
     <row r="52" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="224" t="s">
+      <c r="B52" s="210" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="172" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="226"/>
+      <c r="D52" s="212"/>
       <c r="E52" s="171"/>
       <c r="F52" s="171"/>
       <c r="G52" s="179"/>
@@ -6764,31 +6767,31 @@
       <c r="K52" s="143"/>
       <c r="L52" s="181"/>
       <c r="M52" s="177"/>
-      <c r="N52" s="229" t="s">
+      <c r="N52" s="215" t="s">
         <v>75</v>
       </c>
       <c r="O52" s="182" t="s">
         <v>76</v>
       </c>
-      <c r="P52" s="226"/>
+      <c r="P52" s="212"/>
     </row>
     <row r="53" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="225"/>
+      <c r="B53" s="211"/>
       <c r="C53" s="173" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="225"/>
+      <c r="D53" s="211"/>
       <c r="E53" s="171"/>
       <c r="F53" s="171"/>
       <c r="G53" s="179"/>
       <c r="H53" s="176"/>
       <c r="K53" s="143"/>
       <c r="L53" s="181"/>
-      <c r="N53" s="225"/>
+      <c r="N53" s="211"/>
       <c r="O53" s="165" t="s">
         <v>77</v>
       </c>
-      <c r="P53" s="225"/>
+      <c r="P53" s="211"/>
     </row>
     <row r="54" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="138"/>
@@ -6802,13 +6805,13 @@
       <c r="L54" s="181"/>
     </row>
     <row r="55" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="224" t="s">
+      <c r="B55" s="210" t="s">
         <v>78</v>
       </c>
       <c r="C55" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="226"/>
+      <c r="D55" s="212"/>
       <c r="E55" s="171"/>
       <c r="F55" s="171"/>
       <c r="G55" s="179"/>
@@ -6817,19 +6820,19 @@
       <c r="L55" s="181"/>
     </row>
     <row r="56" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="225"/>
+      <c r="B56" s="211"/>
       <c r="C56" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="225"/>
+      <c r="D56" s="211"/>
       <c r="E56" s="174"/>
-      <c r="F56" s="227" t="s">
+      <c r="F56" s="214" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="H56" s="226"/>
+      <c r="H56" s="212"/>
       <c r="K56" s="143"/>
       <c r="L56" s="181"/>
     </row>
@@ -6837,106 +6840,106 @@
       <c r="B57" s="138"/>
       <c r="D57" s="176"/>
       <c r="E57" s="184"/>
-      <c r="F57" s="225"/>
+      <c r="F57" s="211"/>
       <c r="G57" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="H57" s="225"/>
+      <c r="H57" s="211"/>
       <c r="K57" s="143"/>
       <c r="L57" s="181"/>
     </row>
     <row r="58" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="224" t="s">
+      <c r="B58" s="210" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="226"/>
+      <c r="D58" s="212"/>
       <c r="G58" s="179"/>
       <c r="H58" s="180"/>
       <c r="K58" s="143"/>
       <c r="L58" s="183"/>
     </row>
     <row r="59" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="225"/>
+      <c r="B59" s="211"/>
       <c r="C59" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="225"/>
+      <c r="D59" s="211"/>
       <c r="G59" s="179"/>
       <c r="H59" s="181"/>
       <c r="I59" s="177"/>
-      <c r="J59" s="228" t="s">
+      <c r="J59" s="213" t="s">
         <v>83</v>
       </c>
       <c r="K59" s="182" t="s">
         <v>84</v>
       </c>
-      <c r="L59" s="226"/>
+      <c r="L59" s="212"/>
     </row>
     <row r="60" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="138"/>
       <c r="D60" s="176"/>
       <c r="G60" s="179"/>
       <c r="H60" s="181"/>
-      <c r="J60" s="225"/>
+      <c r="J60" s="211"/>
       <c r="K60" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="L60" s="225"/>
+      <c r="L60" s="211"/>
     </row>
     <row r="61" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="224" t="s">
+      <c r="B61" s="210" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="226"/>
+      <c r="D61" s="212"/>
       <c r="G61" s="179"/>
       <c r="H61" s="183"/>
     </row>
     <row r="62" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="225"/>
+      <c r="B62" s="211"/>
       <c r="C62" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="225"/>
+      <c r="D62" s="211"/>
       <c r="E62" s="174"/>
-      <c r="F62" s="227" t="s">
+      <c r="F62" s="214" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="H62" s="226"/>
+      <c r="H62" s="212"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="138"/>
       <c r="D63" s="176"/>
       <c r="E63" s="184"/>
-      <c r="F63" s="225"/>
+      <c r="F63" s="211"/>
       <c r="G63" s="178" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="225"/>
+      <c r="H63" s="211"/>
     </row>
     <row r="64" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="224" t="s">
+      <c r="B64" s="210" t="s">
         <v>90</v>
       </c>
       <c r="C64" s="172" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="226"/>
+      <c r="D64" s="212"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="225"/>
+      <c r="B65" s="211"/>
       <c r="C65" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="225"/>
+      <c r="D65" s="211"/>
     </row>
     <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7875,37 +7878,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C16:L16"/>
@@ -7920,6 +7892,37 @@
     <mergeCell ref="H39:L40"/>
     <mergeCell ref="D40:G40"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="J59:J60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -7930,8 +7933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:U65"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7949,18 +7952,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="208" t="s">
+      <c r="C2" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" s="77" t="s">
@@ -8179,73 +8182,73 @@
       <c r="L15" s="83"/>
     </row>
     <row r="16" spans="3:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="D16" s="196"/>
+      <c r="E16" s="196"/>
+      <c r="F16" s="196"/>
+      <c r="G16" s="196"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="196"/>
+      <c r="J16" s="196"/>
+      <c r="K16" s="196"/>
+      <c r="L16" s="196"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="209"/>
-      <c r="E17" s="204"/>
-      <c r="F17" s="204"/>
-      <c r="G17" s="205"/>
-      <c r="H17" s="203" t="s">
+      <c r="D17" s="192"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="194"/>
+      <c r="H17" s="199" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="204"/>
-      <c r="J17" s="204"/>
-      <c r="K17" s="204"/>
-      <c r="L17" s="205"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="193"/>
+      <c r="L17" s="194"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="196"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
+      <c r="D18" s="195"/>
+      <c r="E18" s="196"/>
+      <c r="F18" s="196"/>
       <c r="G18" s="197"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="193"/>
-      <c r="J18" s="193"/>
-      <c r="K18" s="193"/>
+      <c r="H18" s="200"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="196"/>
+      <c r="K18" s="196"/>
       <c r="L18" s="197"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="3:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="207" t="s">
+      <c r="C20" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="204"/>
+      <c r="D20" s="193"/>
       <c r="E20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="36"/>
-      <c r="G20" s="207" t="s">
+      <c r="G20" s="201" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="204"/>
+      <c r="H20" s="193"/>
       <c r="I20" s="35" t="s">
         <v>37</v>
       </c>
       <c r="J20" s="36"/>
-      <c r="K20" s="207" t="s">
+      <c r="K20" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="204"/>
+      <c r="L20" s="193"/>
       <c r="M20" s="35" t="s">
         <v>37</v>
       </c>
@@ -8675,47 +8678,47 @@
       <c r="M36" s="92"/>
     </row>
     <row r="38" spans="2:21" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="192" t="s">
+      <c r="C38" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="193"/>
-      <c r="E38" s="193"/>
-      <c r="F38" s="193"/>
-      <c r="G38" s="193"/>
-      <c r="H38" s="193"/>
-      <c r="I38" s="193"/>
-      <c r="J38" s="193"/>
-      <c r="K38" s="193"/>
-      <c r="L38" s="193"/>
+      <c r="D38" s="196"/>
+      <c r="E38" s="196"/>
+      <c r="F38" s="196"/>
+      <c r="G38" s="196"/>
+      <c r="H38" s="196"/>
+      <c r="I38" s="196"/>
+      <c r="J38" s="196"/>
+      <c r="K38" s="196"/>
+      <c r="L38" s="196"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="209"/>
-      <c r="E39" s="204"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="205"/>
-      <c r="H39" s="203" t="s">
+      <c r="D39" s="192"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="194"/>
+      <c r="H39" s="199" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="204"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="205"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
+      <c r="K39" s="193"/>
+      <c r="L39" s="194"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="196"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="193"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="196"/>
+      <c r="F40" s="196"/>
       <c r="G40" s="197"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="193"/>
-      <c r="J40" s="193"/>
-      <c r="K40" s="193"/>
+      <c r="H40" s="200"/>
+      <c r="I40" s="196"/>
+      <c r="J40" s="196"/>
+      <c r="K40" s="196"/>
       <c r="L40" s="197"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
@@ -8723,10 +8726,10 @@
       <c r="C41" s="186"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B42" s="198" t="s">
+      <c r="B42" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="193"/>
+      <c r="C42" s="196"/>
       <c r="D42" s="30" t="s">
         <v>37</v>
       </c>
@@ -8755,73 +8758,77 @@
         <v>37</v>
       </c>
       <c r="Q42" s="39"/>
-      <c r="S42" s="201"/>
-      <c r="T42" s="202"/>
+      <c r="S42" s="198"/>
+      <c r="T42" s="191"/>
       <c r="U42" s="39"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B43" s="190" t="s">
+      <c r="B43" s="207" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="195"/>
+      <c r="D43" s="202" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="44" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="191"/>
+      <c r="B44" s="203"/>
       <c r="C44" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="191"/>
+      <c r="D44" s="203"/>
       <c r="E44" s="44"/>
-      <c r="F44" s="194" t="s">
+      <c r="F44" s="206" t="s">
         <v>63</v>
       </c>
       <c r="G44" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="195"/>
+      <c r="H44" s="202"/>
     </row>
     <row r="45" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="D45" s="93"/>
       <c r="E45" s="43"/>
-      <c r="F45" s="191"/>
+      <c r="F45" s="203"/>
       <c r="G45" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="191"/>
+      <c r="H45" s="203"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B46" s="190" t="s">
+      <c r="B46" s="207" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="195"/>
+      <c r="D46" s="202" t="s">
+        <v>99</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="94"/>
     </row>
     <row r="47" spans="2:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="191"/>
+      <c r="B47" s="203"/>
       <c r="C47" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="191"/>
+      <c r="D47" s="203"/>
       <c r="G47" s="1"/>
       <c r="H47" s="95"/>
       <c r="I47" s="43"/>
-      <c r="J47" s="199" t="s">
+      <c r="J47" s="204" t="s">
         <v>67</v>
       </c>
       <c r="K47" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="L47" s="195"/>
-      <c r="S47" s="201"/>
-      <c r="T47" s="202"/>
+      <c r="L47" s="202"/>
+      <c r="S47" s="198"/>
+      <c r="T47" s="191"/>
       <c r="U47" s="39"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
@@ -8829,39 +8836,41 @@
       <c r="D48" s="93"/>
       <c r="G48" s="1"/>
       <c r="H48" s="95"/>
-      <c r="J48" s="191"/>
+      <c r="J48" s="203"/>
       <c r="K48" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L48" s="191"/>
+      <c r="L48" s="203"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="190" t="s">
+      <c r="B49" s="207" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="195"/>
+      <c r="D49" s="202" t="s">
+        <v>49</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="96"/>
       <c r="K49" s="37"/>
       <c r="L49" s="94"/>
     </row>
     <row r="50" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="191"/>
+      <c r="B50" s="203"/>
       <c r="C50" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="191"/>
+      <c r="D50" s="203"/>
       <c r="E50" s="43"/>
-      <c r="F50" s="194" t="s">
+      <c r="F50" s="206" t="s">
         <v>71</v>
       </c>
       <c r="G50" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H50" s="195"/>
+      <c r="H50" s="202"/>
       <c r="K50" s="37"/>
       <c r="L50" s="95"/>
     </row>
@@ -8869,50 +8878,52 @@
       <c r="B51" s="5"/>
       <c r="D51" s="93"/>
       <c r="E51" s="43"/>
-      <c r="F51" s="191"/>
+      <c r="F51" s="203"/>
       <c r="G51" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="191"/>
+      <c r="H51" s="203"/>
       <c r="K51" s="37"/>
       <c r="L51" s="95"/>
     </row>
     <row r="52" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="190" t="s">
+      <c r="B52" s="207" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="195"/>
+      <c r="D52" s="202" t="s">
+        <v>97</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="93"/>
       <c r="K52" s="37"/>
       <c r="L52" s="95"/>
       <c r="M52" s="43"/>
-      <c r="N52" s="200" t="s">
+      <c r="N52" s="205" t="s">
         <v>75</v>
       </c>
       <c r="O52" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="P52" s="195"/>
+      <c r="P52" s="202"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="191"/>
+      <c r="B53" s="203"/>
       <c r="C53" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="191"/>
+      <c r="D53" s="203"/>
       <c r="G53" s="1"/>
       <c r="H53" s="93"/>
       <c r="K53" s="37"/>
       <c r="L53" s="95"/>
-      <c r="N53" s="191"/>
+      <c r="N53" s="203"/>
       <c r="O53" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="P53" s="191"/>
+      <c r="P53" s="203"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
@@ -8923,32 +8934,34 @@
       <c r="L54" s="95"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="190" t="s">
+      <c r="B55" s="207" t="s">
         <v>78</v>
       </c>
       <c r="C55" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="195"/>
+      <c r="D55" s="202" t="s">
+        <v>47</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="93"/>
       <c r="K55" s="37"/>
       <c r="L55" s="95"/>
     </row>
     <row r="56" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="191"/>
+      <c r="B56" s="203"/>
       <c r="C56" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="191"/>
+      <c r="D56" s="203"/>
       <c r="E56" s="44"/>
-      <c r="F56" s="194" t="s">
+      <c r="F56" s="206" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="H56" s="195"/>
+      <c r="H56" s="202"/>
       <c r="K56" s="37"/>
       <c r="L56" s="95"/>
     </row>
@@ -8956,140 +8969,115 @@
       <c r="B57" s="5"/>
       <c r="D57" s="93"/>
       <c r="E57" s="45"/>
-      <c r="F57" s="191"/>
+      <c r="F57" s="203"/>
       <c r="G57" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="H57" s="191"/>
+      <c r="H57" s="203"/>
       <c r="K57" s="37"/>
       <c r="L57" s="95"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="190" t="s">
+      <c r="B58" s="207" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="195"/>
+      <c r="D58" s="202" t="s">
+        <v>47</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="94"/>
       <c r="K58" s="37"/>
       <c r="L58" s="96"/>
     </row>
     <row r="59" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="191"/>
+      <c r="B59" s="203"/>
       <c r="C59" s="187" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="191"/>
+      <c r="D59" s="203"/>
       <c r="G59" s="1"/>
       <c r="H59" s="95"/>
       <c r="I59" s="43"/>
-      <c r="J59" s="199" t="s">
+      <c r="J59" s="204" t="s">
         <v>83</v>
       </c>
       <c r="K59" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="L59" s="195"/>
+      <c r="L59" s="202"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="D60" s="93"/>
       <c r="G60" s="1"/>
       <c r="H60" s="95"/>
-      <c r="J60" s="191"/>
+      <c r="J60" s="203"/>
       <c r="K60" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="L60" s="191"/>
+      <c r="L60" s="203"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="190" t="s">
+      <c r="B61" s="207" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D61" s="195"/>
+      <c r="D61" s="202" t="s">
+        <v>47</v>
+      </c>
       <c r="G61" s="1"/>
       <c r="H61" s="96"/>
     </row>
     <row r="62" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="191"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="191"/>
+      <c r="D62" s="203"/>
       <c r="E62" s="44"/>
-      <c r="F62" s="194" t="s">
+      <c r="F62" s="206" t="s">
         <v>87</v>
       </c>
       <c r="G62" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="H62" s="195"/>
+      <c r="H62" s="202"/>
     </row>
     <row r="63" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="5"/>
       <c r="D63" s="93"/>
       <c r="E63" s="45"/>
-      <c r="F63" s="191"/>
+      <c r="F63" s="203"/>
       <c r="G63" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="191"/>
+      <c r="H63" s="203"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="190" t="s">
+      <c r="B64" s="207" t="s">
         <v>90</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="195"/>
+      <c r="D64" s="202" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="191"/>
+      <c r="B65" s="203"/>
       <c r="C65" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="191"/>
+      <c r="D65" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C16:L16"/>
@@ -9104,6 +9092,37 @@
     <mergeCell ref="H39:L40"/>
     <mergeCell ref="D40:G40"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="J59:J60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>